<commit_message>
created 4 tables and insert statements for CommentReplies, Topics, PostsWithTopics, and Followers.
</commit_message>
<xml_diff>
--- a/api/db/Sample Data.xlsx
+++ b/api/db/Sample Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\OneDrive\Desktop\Fall 2021\CSE 111\Project\Encapsulate\api\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jstic\Documents\GitHub\Encapsulate\api\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59474335-4EF8-42B1-A8FC-A9AA0BB0E408}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C583DC-2B16-4196-AA59-889FAD87A20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{E22650B2-E1A3-4E24-859B-DDC0275D823A}"/>
+    <workbookView xWindow="2508" yWindow="2508" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="7" xr2:uid="{E22650B2-E1A3-4E24-859B-DDC0275D823A}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -1390,7 +1390,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1530,7 +1530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF6ADBA8-C0BC-47A5-81B2-CF19850FD59B}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1634,7 +1634,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
I added 4 queries & added 4 tables to sqlite db
</commit_message>
<xml_diff>
--- a/api/db/Sample Data.xlsx
+++ b/api/db/Sample Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jstic\Documents\GitHub\Encapsulate\api\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C583DC-2B16-4196-AA59-889FAD87A20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5C2009-A304-49B0-B364-D85A71A18D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2508" yWindow="2508" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="7" xr2:uid="{E22650B2-E1A3-4E24-859B-DDC0275D823A}"/>
+    <workbookView xWindow="2508" yWindow="2508" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="3" xr2:uid="{E22650B2-E1A3-4E24-859B-DDC0275D823A}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -651,7 +651,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -826,7 +826,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1177,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A077CD-F6EF-42C7-A7B7-5F76CAB89EAC}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1774,7 +1774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A34ED8-C26A-463D-837D-7A19BB977673}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modified db values and created queries
</commit_message>
<xml_diff>
--- a/api/db/Sample Data.xlsx
+++ b/api/db/Sample Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jstic\Documents\GitHub\Encapsulate\api\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\OneDrive\Desktop\Fall 2021\CSE 111\Project\Encapsulate\api\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5C2009-A304-49B0-B364-D85A71A18D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2E01B4-C34F-44AB-96F5-3A4E632FA183}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2508" yWindow="2508" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="3" xr2:uid="{E22650B2-E1A3-4E24-859B-DDC0275D823A}"/>
+    <workbookView xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="4" xr2:uid="{E22650B2-E1A3-4E24-859B-DDC0275D823A}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
   <si>
     <t>user_id</t>
   </si>
@@ -275,6 +275,12 @@
   </si>
   <si>
     <t>Sports</t>
+  </si>
+  <si>
+    <t>comment_reply_parent_comment_id</t>
+  </si>
+  <si>
+    <t>comment_reply_date</t>
   </si>
 </sst>
 </file>
@@ -324,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -334,6 +340,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1177,7 +1184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A077CD-F6EF-42C7-A7B7-5F76CAB89EAC}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1387,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E837CAD-F3B4-4365-84F4-C4DF56EB743F}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1398,131 +1405,199 @@
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>37</v>
       </c>
       <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44502</v>
+      </c>
+      <c r="E2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="1">
+        <v>44503</v>
+      </c>
+      <c r="E3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="1">
+        <v>44505</v>
+      </c>
+      <c r="E4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5">
+        <v>44507</v>
+      </c>
+      <c r="E5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5">
+        <v>44509</v>
+      </c>
+      <c r="E6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="5">
+        <v>44510</v>
+      </c>
+      <c r="E7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5">
+        <v>44511</v>
+      </c>
+      <c r="E8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5">
+        <v>44514</v>
+      </c>
+      <c r="E9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3">
+        <v>4</v>
+      </c>
+      <c r="D10" s="5">
+        <v>44518</v>
+      </c>
+      <c r="E10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
+        <v>44520</v>
+      </c>
+      <c r="E11" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>